<commit_message>
Adapt some files to include some Timeslices for CapacityFactor. First, create new sheet Timeslices into A-O_Parametrization.xlsx and populate. Then, change xtra_scen variable into MOMF_T1_A.yaml, specific Timeslice form All to Some.
</commit_message>
<xml_diff>
--- a/t1_confection/A2_Extra_Inputs/A-Xtra_Scenarios.xlsx
+++ b/t1_confection/A2_Extra_Inputs/A-Xtra_Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clgcr.sharepoint.com/sites/ClimateLeadGroup-Decarb_RD/Documentos compartidos/Decarb_RD/WBG/4_Model/RD_Model_v2/A2_Extra_Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A2_Extra_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{EAEA4B35-7A75-46DF-9244-5221D1E50B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{347B2D77-E4EB-449F-BAEA-58072D372812}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269B2C50-3F04-459C-921F-CB1D7D9D542B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Other_Params" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>LTS</t>
+  </si>
+  <si>
+    <t>Timeslices</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
   </si>
 </sst>
 </file>
@@ -137,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -174,7 +186,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -185,7 +199,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -198,7 +214,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -217,6 +235,15 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -224,86 +251,90 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -610,66 +641,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="15" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="C3" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="C4" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
+      <c r="C5" s="13"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
+      <c r="C6" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -688,16 +734,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -928,6 +964,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD3AFD5D-B2EB-4B7C-B9D5-F081DC0BCFEF}">
   <ds:schemaRefs>
@@ -937,6 +983,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70826B31-45BE-4F9C-B5E5-DED838379614}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9422D5EA-73A0-40E6-A4A6-69DD3F347630}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -944,8 +1009,4 @@
     <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70826B31-45BE-4F9C-B5E5-DED838379614}"/>
 </file>
</xml_diff>